<commit_message>
Updates to drug validation in docs.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/DrugsValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/DrugsValidation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\stress_update\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFA7E69-859E-4EC9-80E2-12DC4432825E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3818FEB7-04CE-4FCC-85A1-8EF8DE3FBCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23160" yWindow="8715" windowWidth="33585" windowHeight="21480" tabRatio="736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1590" yWindow="6990" windowWidth="37740" windowHeight="21480" tabRatio="736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="18" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="185">
   <si>
     <t>Event</t>
   </si>
@@ -596,6 +596,9 @@
   </si>
   <si>
     <t xml:space="preserve">Marked Decrease @cite Morgan2006Clinical p200; 25-40% Significant Decrease @cite Kanaya2003differential </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-25% Decrease @cite chase2010model </t>
   </si>
 </sst>
 </file>
@@ -1700,7 +1703,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="K17" sqref="A1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1876,13 +1879,13 @@
         <v>54</v>
       </c>
       <c r="F5" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G5" s="52" t="s">
         <v>94</v>
       </c>
       <c r="H5" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="52" t="s">
         <v>95</v>
@@ -1946,13 +1949,13 @@
         <v>54</v>
       </c>
       <c r="F7" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G7" s="52" t="s">
         <v>94</v>
       </c>
       <c r="H7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="52" t="s">
         <v>95</v>
@@ -2295,14 +2298,14 @@
       </c>
       <c r="F17" s="47">
         <f>SUM(F3:F16)</f>
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G17" s="48" t="s">
         <v>94</v>
       </c>
       <c r="H17" s="49">
         <f>SUM(H3:H16)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I17" s="48" t="s">
         <v>95</v>
@@ -2408,8 +2411,8 @@
   </sheetPr>
   <dimension ref="A2:W14"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2698,9 +2701,9 @@
   <dimension ref="A2:S17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="F4" sqref="F4"/>
-      <selection pane="topRight" activeCell="J16" sqref="J16"/>
+      <selection pane="topRight" activeCell="S17" sqref="A2:S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2718,7 +2721,7 @@
     <col min="11" max="11" width="34.5703125" customWidth="1"/>
     <col min="12" max="12" width="36.7109375" customWidth="1"/>
     <col min="13" max="13" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="52.85546875" customWidth="1"/>
     <col min="15" max="15" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="36.7109375" customWidth="1"/>
     <col min="17" max="17" width="29.7109375" bestFit="1" customWidth="1"/>
@@ -2885,7 +2888,7 @@
         <v>64</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>65</v>
+        <v>184</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>64</v>
@@ -3059,9 +3062,9 @@
         <v>77</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="N7" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" s="14" t="s">
         <v>77</v>
       </c>
       <c r="O7" s="5" t="s">
@@ -4174,7 +4177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D12168-200B-46C7-8F89-55DD217C0DF8}">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>

</xml_diff>